<commit_message>
Output data and touch-ups
</commit_message>
<xml_diff>
--- a/Output Data/Insertion Sort on Ascending Array Results.xlsx
+++ b/Output Data/Insertion Sort on Ascending Array Results.xlsx
@@ -401,7 +401,7 @@
         <v>999.0</v>
       </c>
       <c r="C2" t="n" s="2">
-        <v>2139.0</v>
+        <v>2138.0</v>
       </c>
     </row>
     <row r="3">
@@ -423,7 +423,7 @@
         <v>2999.0</v>
       </c>
       <c r="C4" t="n" s="4">
-        <v>5559.0</v>
+        <v>5560.0</v>
       </c>
     </row>
     <row r="5">
@@ -434,7 +434,7 @@
         <v>3999.0</v>
       </c>
       <c r="C5" t="n" s="5">
-        <v>8553.0</v>
+        <v>6842.0</v>
       </c>
     </row>
     <row r="6">
@@ -445,7 +445,7 @@
         <v>4999.0</v>
       </c>
       <c r="C6" t="n" s="6">
-        <v>14968.0</v>
+        <v>8981.0</v>
       </c>
     </row>
     <row r="7">
@@ -456,7 +456,7 @@
         <v>5999.0</v>
       </c>
       <c r="C7" t="n" s="7">
-        <v>12402.0</v>
+        <v>11974.0</v>
       </c>
     </row>
     <row r="8">
@@ -467,7 +467,7 @@
         <v>6999.0</v>
       </c>
       <c r="C8" t="n" s="8">
-        <v>13257.0</v>
+        <v>12402.0</v>
       </c>
     </row>
     <row r="9">
@@ -478,7 +478,7 @@
         <v>7999.0</v>
       </c>
       <c r="C9" t="n" s="9">
-        <v>21810.0</v>
+        <v>14968.0</v>
       </c>
     </row>
     <row r="10">
@@ -489,7 +489,7 @@
         <v>8999.0</v>
       </c>
       <c r="C10" t="n" s="10">
-        <v>17106.0</v>
+        <v>26087.0</v>
       </c>
     </row>
     <row r="11">
@@ -500,7 +500,7 @@
         <v>9999.0</v>
       </c>
       <c r="C11" t="n" s="11">
-        <v>18816.0</v>
+        <v>40200.0</v>
       </c>
     </row>
     <row r="12">
@@ -511,7 +511,7 @@
         <v>10999.0</v>
       </c>
       <c r="C12" t="n" s="12">
-        <v>20955.0</v>
+        <v>20528.0</v>
       </c>
     </row>
     <row r="13">
@@ -522,7 +522,7 @@
         <v>11999.0</v>
       </c>
       <c r="C13" t="n" s="13">
-        <v>21811.0</v>
+        <v>20955.0</v>
       </c>
     </row>
     <row r="14">
@@ -533,7 +533,7 @@
         <v>12999.0</v>
       </c>
       <c r="C14" t="n" s="14">
-        <v>27370.0</v>
+        <v>25231.0</v>
       </c>
     </row>
     <row r="15">
@@ -544,7 +544,7 @@
         <v>13999.0</v>
       </c>
       <c r="C15" t="n" s="15">
-        <v>40199.0</v>
+        <v>24804.0</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14999.0</v>
       </c>
       <c r="C16" t="n" s="16">
-        <v>28652.0</v>
+        <v>26515.0</v>
       </c>
     </row>
     <row r="17">
@@ -566,7 +566,7 @@
         <v>15999.0</v>
       </c>
       <c r="C17" t="n" s="17">
-        <v>31646.0</v>
+        <v>30363.0</v>
       </c>
     </row>
     <row r="18">
@@ -577,7 +577,7 @@
         <v>16999.0</v>
       </c>
       <c r="C18" t="n" s="18">
-        <v>32929.0</v>
+        <v>30791.0</v>
       </c>
     </row>
     <row r="19">
@@ -588,7 +588,7 @@
         <v>17999.0</v>
       </c>
       <c r="C19" t="n" s="19">
-        <v>34213.0</v>
+        <v>32073.0</v>
       </c>
     </row>
     <row r="20">
@@ -599,7 +599,7 @@
         <v>18999.0</v>
       </c>
       <c r="C20" t="n" s="20">
-        <v>37633.0</v>
+        <v>40199.0</v>
       </c>
     </row>
     <row r="21">
@@ -610,7 +610,7 @@
         <v>19999.0</v>
       </c>
       <c r="C21" t="n" s="21">
-        <v>38916.0</v>
+        <v>41055.0</v>
       </c>
     </row>
     <row r="22">
@@ -621,7 +621,7 @@
         <v>20999.0</v>
       </c>
       <c r="C22" t="n" s="22">
-        <v>44903.0</v>
+        <v>45759.0</v>
       </c>
     </row>
     <row r="23">
@@ -632,7 +632,7 @@
         <v>21999.0</v>
       </c>
       <c r="C23" t="n" s="23">
-        <v>43620.0</v>
+        <v>42338.0</v>
       </c>
     </row>
     <row r="24">
@@ -643,7 +643,7 @@
         <v>22999.0</v>
       </c>
       <c r="C24" t="n" s="24">
-        <v>67997.0</v>
+        <v>47042.0</v>
       </c>
     </row>
     <row r="25">
@@ -654,7 +654,7 @@
         <v>23999.0</v>
       </c>
       <c r="C25" t="n" s="25">
-        <v>49608.0</v>
+        <v>60299.0</v>
       </c>
     </row>
     <row r="26">
@@ -665,7 +665,7 @@
         <v>24999.0</v>
       </c>
       <c r="C26" t="n" s="26">
-        <v>50036.0</v>
+        <v>53457.0</v>
       </c>
     </row>
     <row r="27">
@@ -676,7 +676,7 @@
         <v>25999.0</v>
       </c>
       <c r="C27" t="n" s="27">
-        <v>55595.0</v>
+        <v>51319.0</v>
       </c>
     </row>
     <row r="28">
@@ -687,7 +687,7 @@
         <v>26999.0</v>
       </c>
       <c r="C28" t="n" s="28">
-        <v>59444.0</v>
+        <v>55167.0</v>
       </c>
     </row>
     <row r="29">
@@ -698,7 +698,7 @@
         <v>27999.0</v>
       </c>
       <c r="C29" t="n" s="29">
-        <v>53029.0</v>
+        <v>53884.0</v>
       </c>
     </row>
     <row r="30">
@@ -709,7 +709,7 @@
         <v>28999.0</v>
       </c>
       <c r="C30" t="n" s="30">
-        <v>61582.0</v>
+        <v>54312.0</v>
       </c>
     </row>
     <row r="31">
@@ -720,7 +720,7 @@
         <v>29999.0</v>
       </c>
       <c r="C31" t="n" s="31">
-        <v>63293.0</v>
+        <v>56878.0</v>
       </c>
     </row>
     <row r="32">
@@ -731,7 +731,7 @@
         <v>30999.0</v>
       </c>
       <c r="C32" t="n" s="32">
-        <v>70135.0</v>
+        <v>54740.0</v>
       </c>
     </row>
     <row r="33">
@@ -742,7 +742,7 @@
         <v>31999.0</v>
       </c>
       <c r="C33" t="n" s="33">
-        <v>68425.0</v>
+        <v>63720.0</v>
       </c>
     </row>
     <row r="34">
@@ -753,7 +753,7 @@
         <v>32999.0</v>
       </c>
       <c r="C34" t="n" s="34">
-        <v>68424.0</v>
+        <v>68425.0</v>
       </c>
     </row>
     <row r="35">
@@ -764,7 +764,7 @@
         <v>33999.0</v>
       </c>
       <c r="C35" t="n" s="35">
-        <v>65858.0</v>
+        <v>85103.0</v>
       </c>
     </row>
     <row r="36">
@@ -775,7 +775,7 @@
         <v>34999.0</v>
       </c>
       <c r="C36" t="n" s="36">
-        <v>73128.0</v>
+        <v>64575.0</v>
       </c>
     </row>
     <row r="37">
@@ -786,7 +786,7 @@
         <v>35999.0</v>
       </c>
       <c r="C37" t="n" s="37">
-        <v>70990.0</v>
+        <v>75694.0</v>
       </c>
     </row>
     <row r="38">
@@ -797,7 +797,7 @@
         <v>36999.0</v>
       </c>
       <c r="C38" t="n" s="38">
-        <v>78688.0</v>
+        <v>77833.0</v>
       </c>
     </row>
     <row r="39">
@@ -808,7 +808,7 @@
         <v>37999.0</v>
       </c>
       <c r="C39" t="n" s="39">
-        <v>76978.0</v>
+        <v>78260.0</v>
       </c>
     </row>
     <row r="40">
@@ -819,7 +819,7 @@
         <v>38999.0</v>
       </c>
       <c r="C40" t="n" s="40">
-        <v>79971.0</v>
+        <v>73556.0</v>
       </c>
     </row>
     <row r="41">
@@ -830,7 +830,7 @@
         <v>39999.0</v>
       </c>
       <c r="C41" t="n" s="41">
-        <v>76122.0</v>
+        <v>82964.0</v>
       </c>
     </row>
     <row r="42">
@@ -841,7 +841,7 @@
         <v>40999.0</v>
       </c>
       <c r="C42" t="n" s="42">
-        <v>87241.0</v>
+        <v>90235.0</v>
       </c>
     </row>
     <row r="43">
@@ -852,7 +852,7 @@
         <v>41999.0</v>
       </c>
       <c r="C43" t="n" s="43">
-        <v>84247.0</v>
+        <v>118460.0</v>
       </c>
     </row>
     <row r="44">
@@ -863,7 +863,7 @@
         <v>42999.0</v>
       </c>
       <c r="C44" t="n" s="44">
-        <v>127441.0</v>
+        <v>82110.0</v>
       </c>
     </row>
     <row r="45">
@@ -874,7 +874,7 @@
         <v>43999.0</v>
       </c>
       <c r="C45" t="n" s="45">
-        <v>84675.0</v>
+        <v>90234.0</v>
       </c>
     </row>
     <row r="46">
@@ -885,7 +885,7 @@
         <v>44999.0</v>
       </c>
       <c r="C46" t="n" s="46">
-        <v>92801.0</v>
+        <v>91090.0</v>
       </c>
     </row>
     <row r="47">
@@ -896,7 +896,7 @@
         <v>45999.0</v>
       </c>
       <c r="C47" t="n" s="47">
-        <v>91518.0</v>
+        <v>98788.0</v>
       </c>
     </row>
     <row r="48">
@@ -907,7 +907,7 @@
         <v>46999.0</v>
       </c>
       <c r="C48" t="n" s="48">
-        <v>96649.0</v>
+        <v>91945.0</v>
       </c>
     </row>
     <row r="49">
@@ -918,7 +918,7 @@
         <v>47999.0</v>
       </c>
       <c r="C49" t="n" s="49">
-        <v>97505.0</v>
+        <v>97077.0</v>
       </c>
     </row>
     <row r="50">
@@ -929,7 +929,7 @@
         <v>48999.0</v>
       </c>
       <c r="C50" t="n" s="50">
-        <v>100498.0</v>
+        <v>93229.0</v>
       </c>
     </row>
     <row r="51">
@@ -940,7 +940,7 @@
         <v>49999.0</v>
       </c>
       <c r="C51" t="n" s="51">
-        <v>97932.0</v>
+        <v>91090.0</v>
       </c>
     </row>
     <row r="52">
@@ -951,7 +951,7 @@
         <v>50999.0</v>
       </c>
       <c r="C52" t="n" s="52">
-        <v>100926.0</v>
+        <v>99215.0</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         <v>51999.0</v>
       </c>
       <c r="C53" t="n" s="53">
-        <v>154810.0</v>
+        <v>98788.0</v>
       </c>
     </row>
     <row r="54">
@@ -973,7 +973,7 @@
         <v>52999.0</v>
       </c>
       <c r="C54" t="n" s="54">
-        <v>106913.0</v>
+        <v>100498.0</v>
       </c>
     </row>
     <row r="55">
@@ -984,7 +984,7 @@
         <v>53999.0</v>
       </c>
       <c r="C55" t="n" s="55">
-        <v>103920.0</v>
+        <v>101781.0</v>
       </c>
     </row>
     <row r="56">
@@ -995,7 +995,7 @@
         <v>54999.0</v>
       </c>
       <c r="C56" t="n" s="56">
-        <v>110335.0</v>
+        <v>102209.0</v>
       </c>
     </row>
     <row r="57">
@@ -1006,7 +1006,7 @@
         <v>55999.0</v>
       </c>
       <c r="C57" t="n" s="57">
-        <v>118887.0</v>
+        <v>107341.0</v>
       </c>
     </row>
     <row r="58">
@@ -1017,7 +1017,7 @@
         <v>56999.0</v>
       </c>
       <c r="C58" t="n" s="58">
-        <v>109907.0</v>
+        <v>108197.0</v>
       </c>
     </row>
     <row r="59">
@@ -1028,7 +1028,7 @@
         <v>57999.0</v>
       </c>
       <c r="C59" t="n" s="59">
-        <v>125302.0</v>
+        <v>108197.0</v>
       </c>
     </row>
     <row r="60">
@@ -1039,7 +1039,7 @@
         <v>58999.0</v>
       </c>
       <c r="C60" t="n" s="60">
-        <v>124875.0</v>
+        <v>108624.0</v>
       </c>
     </row>
     <row r="61">
@@ -1050,7 +1050,7 @@
         <v>59999.0</v>
       </c>
       <c r="C61" t="n" s="61">
-        <v>123164.0</v>
+        <v>116750.0</v>
       </c>
     </row>
     <row r="62">
@@ -1061,7 +1061,7 @@
         <v>60999.0</v>
       </c>
       <c r="C62" t="n" s="62">
-        <v>123164.0</v>
+        <v>119743.0</v>
       </c>
     </row>
     <row r="63">
@@ -1072,7 +1072,7 @@
         <v>61999.0</v>
       </c>
       <c r="C63" t="n" s="63">
-        <v>127013.0</v>
+        <v>111617.0</v>
       </c>
     </row>
     <row r="64">
@@ -1083,7 +1083,7 @@
         <v>62999.0</v>
       </c>
       <c r="C64" t="n" s="64">
-        <v>138559.0</v>
+        <v>124875.0</v>
       </c>
     </row>
     <row r="65">
@@ -1094,7 +1094,7 @@
         <v>63999.0</v>
       </c>
       <c r="C65" t="n" s="65">
-        <v>136422.0</v>
+        <v>122309.0</v>
       </c>
     </row>
     <row r="66">
@@ -1105,7 +1105,7 @@
         <v>64999.0</v>
       </c>
       <c r="C66" t="n" s="66">
-        <v>131290.0</v>
+        <v>125302.0</v>
       </c>
     </row>
     <row r="67">
@@ -1116,7 +1116,7 @@
         <v>65999.0</v>
       </c>
       <c r="C67" t="n" s="67">
-        <v>134711.0</v>
+        <v>124019.0</v>
       </c>
     </row>
     <row r="68">
@@ -1127,7 +1127,7 @@
         <v>66999.0</v>
       </c>
       <c r="C68" t="n" s="68">
-        <v>149678.0</v>
+        <v>128296.0</v>
       </c>
     </row>
     <row r="69">
@@ -1138,7 +1138,7 @@
         <v>67999.0</v>
       </c>
       <c r="C69" t="n" s="69">
-        <v>138559.0</v>
+        <v>134283.0</v>
       </c>
     </row>
     <row r="70">
@@ -1149,7 +1149,7 @@
         <v>68999.0</v>
       </c>
       <c r="C70" t="n" s="70">
-        <v>144974.0</v>
+        <v>137704.0</v>
       </c>
     </row>
     <row r="71">
@@ -1160,7 +1160,7 @@
         <v>69999.0</v>
       </c>
       <c r="C71" t="n" s="71">
-        <v>144119.0</v>
+        <v>131289.0</v>
       </c>
     </row>
     <row r="72">
@@ -1171,7 +1171,7 @@
         <v>70999.0</v>
       </c>
       <c r="C72" t="n" s="72">
-        <v>146685.0</v>
+        <v>131717.0</v>
       </c>
     </row>
     <row r="73">
@@ -1182,7 +1182,7 @@
         <v>71999.0</v>
       </c>
       <c r="C73" t="n" s="73">
-        <v>155238.0</v>
+        <v>139415.0</v>
       </c>
     </row>
     <row r="74">
@@ -1193,7 +1193,7 @@
         <v>72999.0</v>
       </c>
       <c r="C74" t="n" s="74">
-        <v>148396.0</v>
+        <v>137704.0</v>
       </c>
     </row>
     <row r="75">
@@ -1204,7 +1204,7 @@
         <v>73999.0</v>
       </c>
       <c r="C75" t="n" s="75">
-        <v>154382.0</v>
+        <v>143691.0</v>
       </c>
     </row>
     <row r="76">
@@ -1215,7 +1215,7 @@
         <v>74999.0</v>
       </c>
       <c r="C76" t="n" s="76">
-        <v>155238.0</v>
+        <v>144118.0</v>
       </c>
     </row>
     <row r="77">
@@ -1226,7 +1226,7 @@
         <v>75999.0</v>
       </c>
       <c r="C77" t="n" s="77">
-        <v>151817.0</v>
+        <v>144547.0</v>
       </c>
     </row>
     <row r="78">
@@ -1237,7 +1237,7 @@
         <v>76999.0</v>
       </c>
       <c r="C78" t="n" s="78">
-        <v>155665.0</v>
+        <v>146685.0</v>
       </c>
     </row>
     <row r="79">
@@ -1248,7 +1248,7 @@
         <v>77999.0</v>
       </c>
       <c r="C79" t="n" s="79">
-        <v>156949.0</v>
+        <v>145402.0</v>
       </c>
     </row>
     <row r="80">
@@ -1259,7 +1259,7 @@
         <v>78999.0</v>
       </c>
       <c r="C80" t="n" s="80">
-        <v>167640.0</v>
+        <v>148823.0</v>
       </c>
     </row>
     <row r="81">
@@ -1270,7 +1270,7 @@
         <v>79999.0</v>
       </c>
       <c r="C81" t="n" s="81">
-        <v>161653.0</v>
+        <v>202279.0</v>
       </c>
     </row>
     <row r="82">
@@ -1281,7 +1281,7 @@
         <v>80999.0</v>
       </c>
       <c r="C82" t="n" s="82">
-        <v>155665.0</v>
+        <v>155666.0</v>
       </c>
     </row>
     <row r="83">
@@ -1292,7 +1292,7 @@
         <v>81999.0</v>
       </c>
       <c r="C83" t="n" s="83">
-        <v>171917.0</v>
+        <v>148396.0</v>
       </c>
     </row>
     <row r="84">
@@ -1303,7 +1303,7 @@
         <v>82999.0</v>
       </c>
       <c r="C84" t="n" s="84">
-        <v>171489.0</v>
+        <v>158660.0</v>
       </c>
     </row>
     <row r="85">
@@ -1314,7 +1314,7 @@
         <v>83999.0</v>
       </c>
       <c r="C85" t="n" s="85">
-        <v>171061.0</v>
+        <v>159087.0</v>
       </c>
     </row>
     <row r="86">
@@ -1325,7 +1325,7 @@
         <v>84999.0</v>
       </c>
       <c r="C86" t="n" s="86">
-        <v>165074.0</v>
+        <v>169778.0</v>
       </c>
     </row>
     <row r="87">
@@ -1336,7 +1336,7 @@
         <v>85999.0</v>
       </c>
       <c r="C87" t="n" s="87">
-        <v>179615.0</v>
+        <v>176620.0</v>
       </c>
     </row>
     <row r="88">
@@ -1347,7 +1347,7 @@
         <v>86999.0</v>
       </c>
       <c r="C88" t="n" s="88">
-        <v>171489.0</v>
+        <v>165074.0</v>
       </c>
     </row>
     <row r="89">
@@ -1358,7 +1358,7 @@
         <v>87999.0</v>
       </c>
       <c r="C89" t="n" s="89">
-        <v>173200.0</v>
+        <v>237347.0</v>
       </c>
     </row>
     <row r="90">
@@ -1369,7 +1369,7 @@
         <v>88999.0</v>
       </c>
       <c r="C90" t="n" s="90">
-        <v>183891.0</v>
+        <v>169778.0</v>
       </c>
     </row>
     <row r="91">
@@ -1380,7 +1380,7 @@
         <v>89999.0</v>
       </c>
       <c r="C91" t="n" s="91">
-        <v>178331.0</v>
+        <v>163363.0</v>
       </c>
     </row>
     <row r="92">
@@ -1391,7 +1391,7 @@
         <v>90999.0</v>
       </c>
       <c r="C92" t="n" s="92">
-        <v>183036.0</v>
+        <v>175766.0</v>
       </c>
     </row>
     <row r="93">
@@ -1402,7 +1402,7 @@
         <v>91999.0</v>
       </c>
       <c r="C93" t="n" s="93">
-        <v>210833.0</v>
+        <v>169778.0</v>
       </c>
     </row>
     <row r="94">
@@ -1413,7 +1413,7 @@
         <v>92999.0</v>
       </c>
       <c r="C94" t="n" s="94">
-        <v>193299.0</v>
+        <v>177476.0</v>
       </c>
     </row>
     <row r="95">
@@ -1424,7 +1424,7 @@
         <v>93999.0</v>
       </c>
       <c r="C95" t="n" s="95">
-        <v>193727.0</v>
+        <v>174910.0</v>
       </c>
     </row>
     <row r="96">
@@ -1435,7 +1435,7 @@
         <v>94999.0</v>
       </c>
       <c r="C96" t="n" s="96">
-        <v>186456.0</v>
+        <v>170633.0</v>
       </c>
     </row>
     <row r="97">
@@ -1446,7 +1446,7 @@
         <v>95999.0</v>
       </c>
       <c r="C97" t="n" s="97">
-        <v>185602.0</v>
+        <v>181753.0</v>
       </c>
     </row>
     <row r="98">
@@ -1457,7 +1457,7 @@
         <v>96999.0</v>
       </c>
       <c r="C98" t="n" s="98">
-        <v>184319.0</v>
+        <v>180042.0</v>
       </c>
     </row>
     <row r="99">
@@ -1468,7 +1468,7 @@
         <v>97999.0</v>
       </c>
       <c r="C99" t="n" s="99">
-        <v>180042.0</v>
+        <v>217675.0</v>
       </c>
     </row>
     <row r="100">
@@ -1479,7 +1479,7 @@
         <v>98999.0</v>
       </c>
       <c r="C100" t="n" s="100">
-        <v>259585.0</v>
+        <v>206556.0</v>
       </c>
     </row>
     <row r="101">
@@ -1490,7 +1490,7 @@
         <v>99999.0</v>
       </c>
       <c r="C101" t="n" s="101">
-        <v>198003.0</v>
+        <v>193299.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>